<commit_message>
Added C3DC scripts to existing framework
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC01_C3DC_phs002599_SexAtBirth-Female.xlsx
+++ b/InputFiles/C3DC/TC01_C3DC_phs002599_SexAtBirth-Female.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAD871C-80DB-C649-BB23-E4293809BEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61145DD0-BBCD-5243-AE2F-CBDCCC390530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41180" yWindow="220" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="37500" yWindow="2700" windowWidth="30240" windowHeight="17920" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>WebExcel</t>
   </si>
@@ -47,12 +47,6 @@
     <t>TabName</t>
   </si>
   <si>
-    <t>SamplesTab</t>
-  </si>
-  <si>
-    <t>FilesTab</t>
-  </si>
-  <si>
     <t>ParticipantsTab</t>
   </si>
   <si>
@@ -65,152 +59,35 @@
     <t>DiagnosisTab</t>
   </si>
   <si>
-    <t>StudiesTab</t>
-  </si>
-  <si>
-    <t>SELECT
-    st.study_short_title AS "Study Short Title",
-    st.study_id AS "Study ID",
-    diag.diagnosis_classification AS "Diagnosis (Top 5)",
-    COUNT(diag.anatomic_site) AS "Diagnosis Anatomic Site (Top 5)",
-    COUNT(DISTINCT p.participant_id) AS "Number of Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Number of Samples",
-    COUNT(DISTINCT sqf.sequencing_file_id) AS "Number of Files",
-    GROUP_CONCAT(DISTINCT sqf.file_type) AS "File Type (Top 5)",
-    GROUP_CONCAT(DISTINCT pub.pubmed_id) AS "PubMed ID",
-    sp.personnel_name AS "Principal Investigator(s)",
-    sf.grant_id AS "Grant ID"
+    <t>TC01_C3DC_phs002599_SexAtBirth-Female_TSVData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_C3DC_phs002599_SexAtBirth-Female_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>SELECT 
+    COUNT(DISTINCT dgn.diagnosis) AS Diagnoses,
+    COUNT(DISTINCT prt.participant_id) AS Participants,
+    COUNT(DISTINCT std.study_id) AS Studies
 FROM 
-    df_study st
-JOIN 
-    df_participant p ON p."study.id" = st.id
-LEFT JOIN 
-    df_sample smp ON smp."participant.id" = p.participant_id
-LEFT JOIN 
-    df_diagnosis diag ON diag."participant.id" = p.participant_id
-LEFT JOIN 
-    df_publication pub ON pub."study.id" = st.study_id
-LEFT JOIN 
-    df_sequencing_file sqf ON sqf."sample.id" = smp.sample_id
-LEFT JOIN 
-    df_study_personnel sp ON sp."study.id" = st.study_id
-LEFT JOIN 
-    df_study_funding sf ON sf."study.id" = st.study_id
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    st.study_id = 'phs002504' AND p.sex_at_birth = 'Male'
-GROUP BY 
-    st.study_short_title, st.study_id, sf.grant_id
-ORDER BY 
-    st.study_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT
-    p.participant_id AS "Participant ID",
-    st.study_id AS "Study ID",
-    COALESCE(diag.diagnosis_classification, '') AS "Diagnosis",
-    COALESCE(diag.anatomic_site, '') AS "Diagnosis Anatomic Site",
-    COALESCE(diag.diagnosis_classification_system, '') AS "Diagnosis Classification System",
-    COALESCE(diag.diagnosis_verification_status, '') AS "Diagnosis Verification Status",
-    COALESCE(diag.diagnosis_basis, '') AS "Diagnosis Basis",
-    COALESCE(diag.diagnosis_comment, '') AS "Diagnosis Comment",
-    COALESCE(diag.disease_phase, '') AS "Disease Phase",
-    COALESCE(CASE WHEN diag.age_at_diagnosis = -999 THEN 'Not Reported' ELSE diag.age_at_diagnosis END, 0) AS "Age at Diagnosis (days)",
-    COALESCE(fu.vital_status, '') AS "Vital Status"
-FROM 
-    df_participant p
-JOIN 
-    df_study st ON p."study.id" = st.id
-LEFT JOIN 
-    df_diagnosis diag ON diag."participant.id" = p.id
-LEFT JOIN 
-    df_follow_up fu ON fu."participant.id" = p.id
-WHERE 
-    st.study_id = 'phs002504' AND p.sex_at_birth = 'Male'
-ORDER BY 
-    p.participant_id ASC
-LIMIT 100;</t>
+    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female';</t>
   </si>
   <si>
     <t>SELECT DISTINCT
-    smp.sample_id AS "Sample ID",
-    p.participant_id AS "Participant ID",
-    st.study_id AS "Study ID",
-    smp.anatomic_site AS "Sample Anatomic Site",
-    COALESCE(CASE WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' ELSE smp.participant_age_at_collection END, 0) AS "Age at Sample Collection (days)",
-    COALESCE(diag.diagnosis_classification, '') AS "Diagnosis",
-    COALESCE(diag.diagnosis_classification_system, '') AS "Diagnosis Classification System",
-    COALESCE(diag.diagnosis_verification_status, '') AS "Diagnosis Verification Status",
-    COALESCE(diag.diagnosis_basis, '') AS "Diagnosis Basis",
-    COALESCE(diag.diagnosis_comment, '') AS "Diagnosis Comment",
-    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification"
-FROM 
-    df_participant p
-JOIN 
-    df_study st ON p."study.id" = st.id
-LEFT JOIN 
-    df_sample smp ON smp."participant.id" = p.id
-LEFT JOIN 
-    df_diagnosis diag ON diag."participant.id" = p.id
-LEFT JOIN 
-    df_follow_up fu ON fu."participant.id" = p.id
-LEFT JOIN 
-    df_publication pub ON pub."study.id" = st.study_id
-LEFT JOIN 
-    df_sequencing_file sqf ON sqf."sample.id" = smp.sample_id
-WHERE 
-    st.study_id = 'phs002504' AND p.sex_at_birth = 'Male' AND smp.sample_id IS NOT NULL
-ORDER BY 
-    smp.sample_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    sqf.file_name AS "File Name",
-    --sqf.file_category AS "File Category",
-    COALESCE(sqf.file_description, '') AS "File Description",
-    sqf.file_type AS "File Type",
-    CASE     
-    WHEN sqf.file_size &gt;= 1024 * 1024 * 1024 THEN 
-        ROUND(sqf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
-    WHEN sqf.file_size &gt;= 1024 * 1024 THEN 
-        ROUND(sqf.file_size / (1024.0 * 1024.0), 2) || ' MB' 
-    WHEN sqf.file_size &gt;= 1024 THEN 
-        ROUND(sqf.file_size / 1024.0, 2) || ' KB' 
-    ELSE 
-        ROUND(sqf.file_size, 2) || ' Bytes' 
-END AS "File Size",
-    st.study_id AS "Study ID",
-    p.participant_id AS "Participant ID",
-    smp.sample_id AS "Sample ID",
-    sqf.dcf_indexd_guid AS "GUID",
-    sqf.md5sum AS "MD5sum",
-    COALESCE(sqf.library_selection, '') AS "Library Selection",
-    COALESCE(sqf.library_source, '') AS "Library Source",
-    COALESCE(sqf.library_strategy, '') AS "Library Strategy"
-FROM 
-    df_sequencing_file sqf
-LEFT JOIN 
-    df_sample smp ON sqf."sample.id" = smp.id
-LEFT JOIN 
-    df_participant p ON smp."participant.id" = p.id
-LEFT JOIN 
-    df_study st ON p."study.id" = st.id
-WHERE 
-    st.study_id = 'phs002504' AND p.sex_at_birth = 'Male'
-ORDER BY 
-    sqf.file_name ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>TC01_C3DC_phs002599_SexAtBirth-Female_TSVData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_C3DC_phs002599_SexAtBirth-Female_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>SELECT 
     prt.participant_id AS "Participant Id",
     prt.race AS "Race",
     prt.sex_at_birth AS "Sex at Birth",
@@ -218,29 +95,43 @@
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.study_id = prt"prt.study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.participant_id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.participant_id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.participant_id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.participant_id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.study_id = rfs."study.id"
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.study_id = 'phs002599' AND prt.sex_at_birth = 'Female';</t>
-  </si>
-  <si>
-    <t>SELECT 
-    COUNT(DISTINCT dgn.diagnosis_id) AS Diagnoses,
-    COUNT(DISTINCT prt.participant_id) AS Participants,
-    COUNT(DISTINCT std.study_id) AS Studies
+    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female'
+ORDER BY 
+    prt.participant_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    prt.participant_id AS "Participant Id",
+    dgn.diagnosis AS "Diagnosis",
+    dgn.diagnosis_classification_system AS "Diagnosis Classification System",
+    dgn.diagnosis_basis AS "Diagnosis Basis",
+    dgn.tumor_classification AS "Tumor Classification",
+    dgn.anatomic_site AS "Anatomic Site",
+    CASE 
+    WHEN dgn.age_at_diagnosis = -999 THEN 'Not Reported'
+    WHEN dgn.age_at_diagnosis &gt;= 1000 THEN 
+        substr(dgn.age_at_diagnosis, 1, length(dgn.age_at_diagnosis) - 3) || ',' || substr(dgn.age_at_diagnosis, -3)
+    ELSE 
+        dgn.age_at_diagnosis 
+END AS "Age at Diagnosis (days)",
+    std.dbgap_accession AS "dbGaP Accession"
 FROM 
     df_study std
 LEFT JOIN 
-    df_participant prt ON std.id = "prt.study.id"
+    df_participant prt ON std.id = prt."study.id"
 LEFT JOIN 
     df_diagnoses dgn ON prt.id = dgn."participant.id"
 LEFT JOIN 
@@ -252,14 +143,144 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.study_id = 'phs002599' AND prt.sex_at_birth = 'Female';</t>
+    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female'
+ORDER BY 
+    prt.participant_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SurvivalTab</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    prt.participant_id AS "Participant Id",
+    srv.last_known_survival_status AS "Last Known Survival Status",
+    CASE 
+    WHEN srv.age_at_last_known_survival_status = -999 THEN 'Not Reported'
+    WHEN srv.age_at_last_known_survival_status &gt;= 1000 THEN 
+        substr(srv.age_at_last_known_survival_status, 1, length(srv.age_at_last_known_survival_status) - 3) || ',' || substr(srv.age_at_last_known_survival_status, -3)
+    ELSE 
+        srv.age_at_last_known_survival_status 
+END AS "Age at Last Known Survival Status",
+    srv.first_event AS "First Event",
+    std.dbgap_accession AS "dbGaP Accession"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female';</t>
+  </si>
+  <si>
+    <t>StudiesTab</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+     std.dbgap_accession AS "dbGaP Accession",
+     std.study_name AS "Study Name"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female';</t>
+  </si>
+  <si>
+    <t>TreatmentTab</t>
+  </si>
+  <si>
+    <t>TreatmentRespTab</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    prt.participant_id AS "Participant Id",
+    trr.treatment_response_id AS "Treatment Response Id",
+    trr.response AS "Response",
+    CASE 
+        WHEN trr.age_at_response = -999 THEN 'Not Reported'
+        WHEN trr.age_at_response &gt;= 1000 THEN 
+            substr(trr.age_at_response, 1, length(trr.age_at_response) - 3) || ',' || substr(trr.age_at_response, -3)
+        ELSE 
+            trr.age_at_response 
+    END AS "Age at Response",
+    trr.response_category AS "Response Category",
+    trr.response_system AS "Response System",
+    std.dbgap_accession AS "dbGaP Accession"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female'
+ORDER BY 
+    prt.participant_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    prt.participant_id AS "Participant ID",
+    trt.treatment_id AS "Treatment ID",
+    trt.age_at_treatment_start AS "Age at Treatment Start",
+    trt.age_at_treatment_end AS "Age at Treatment End",
+    trt.treatment_type AS "Treatment Type",
+    trt.treatment_agent AS "Treatment Agent",
+    std.dbgap_accession AS "dbGaP Accession"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female'
+ORDER BY 
+    prt.participant_id ASC
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,13 +336,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -344,12 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -682,18 +693,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.83203125" customWidth="1"/>
-    <col min="4" max="4" width="70.1640625" customWidth="1"/>
-    <col min="5" max="5" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="75.83203125" customWidth="1"/>
+    <col min="3" max="3" width="60.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -701,77 +713,85 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="356" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="372" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+    <row r="7" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>

<commit_message>
Added INS framework code and 4 testcases
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC01_C3DC_phs002599_SexAtBirth-Female.xlsx
+++ b/InputFiles/C3DC/TC01_C3DC_phs002599_SexAtBirth-Female.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61145DD0-BBCD-5243-AE2F-CBDCCC390530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0EB55F-53C6-4A41-A7FC-CF85EA649A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37500" yWindow="2700" windowWidth="30240" windowHeight="17920" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -113,73 +113,7 @@
 LIMIT 100;</t>
   </si>
   <si>
-    <t>SELECT DISTINCT
-    prt.participant_id AS "Participant Id",
-    dgn.diagnosis AS "Diagnosis",
-    dgn.diagnosis_classification_system AS "Diagnosis Classification System",
-    dgn.diagnosis_basis AS "Diagnosis Basis",
-    dgn.tumor_classification AS "Tumor Classification",
-    dgn.anatomic_site AS "Anatomic Site",
-    CASE 
-    WHEN dgn.age_at_diagnosis = -999 THEN 'Not Reported'
-    WHEN dgn.age_at_diagnosis &gt;= 1000 THEN 
-        substr(dgn.age_at_diagnosis, 1, length(dgn.age_at_diagnosis) - 3) || ',' || substr(dgn.age_at_diagnosis, -3)
-    ELSE 
-        dgn.age_at_diagnosis 
-END AS "Age at Diagnosis (days)",
-    std.dbgap_accession AS "dbGaP Accession"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
-WHERE 
-    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female'
-ORDER BY 
-    prt.participant_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
     <t>SurvivalTab</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    prt.participant_id AS "Participant Id",
-    srv.last_known_survival_status AS "Last Known Survival Status",
-    CASE 
-    WHEN srv.age_at_last_known_survival_status = -999 THEN 'Not Reported'
-    WHEN srv.age_at_last_known_survival_status &gt;= 1000 THEN 
-        substr(srv.age_at_last_known_survival_status, 1, length(srv.age_at_last_known_survival_status) - 3) || ',' || substr(srv.age_at_last_known_survival_status, -3)
-    ELSE 
-        srv.age_at_last_known_survival_status 
-END AS "Age at Last Known Survival Status",
-    srv.first_event AS "First Event",
-    std.dbgap_accession AS "dbGaP Accession"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
-WHERE 
-    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female';</t>
   </si>
   <si>
     <t>StudiesTab</t>
@@ -248,12 +182,20 @@
   </si>
   <si>
     <t>SELECT DISTINCT
-    prt.participant_id AS "Participant ID",
-    trt.treatment_id AS "Treatment ID",
-    trt.age_at_treatment_start AS "Age at Treatment Start",
-    trt.age_at_treatment_end AS "Age at Treatment End",
-    trt.treatment_type AS "Treatment Type",
-    trt.treatment_agent AS "Treatment Agent",
+    prt.participant_id AS "Participant Id",
+    dgn.diagnosis_id AS "Diagnosis Id",
+    dgn.diagnosis AS "Diagnosis",
+    dgn.diagnosis_classification_system AS "Diagnosis Classification System",
+    dgn.diagnosis_basis AS "Diagnosis Basis",
+    dgn.tumor_classification AS "Tumor Classification",
+    dgn.anatomic_site AS "Anatomic Site",
+    CASE 
+    WHEN dgn.age_at_diagnosis = -999 THEN 'Not Reported'
+    WHEN dgn.age_at_diagnosis &gt;= 1000 THEN 
+        substr(dgn.age_at_diagnosis, 1, length(dgn.age_at_diagnosis) - 3) || ',' || substr(dgn.age_at_diagnosis, -3)
+    ELSE 
+        dgn.age_at_diagnosis 
+END AS "Age at Diagnosis (days)",
     std.dbgap_accession AS "dbGaP Accession"
 FROM 
     df_study std
@@ -275,21 +217,75 @@
     prt.participant_id ASC
 LIMIT 100;</t>
   </si>
+  <si>
+    <t>SELECT DISTINCT
+    prt.participant_id AS "Participant Id",
+    srv.survival_id AS "Survival Id",
+    srv.last_known_survival_status AS "Last Known Survival Status",
+    CASE 
+    WHEN srv.age_at_last_known_survival_status = -999 THEN 'Not Reported'
+    WHEN srv.age_at_last_known_survival_status &gt;= 1000 THEN 
+        substr(srv.age_at_last_known_survival_status, 1, length(srv.age_at_last_known_survival_status) - 3) || ',' || substr(srv.age_at_last_known_survival_status, -3)
+    ELSE 
+        srv.age_at_last_known_survival_status 
+END AS "Age at Last Known Survival Status",
+    srv.first_event AS "First Event",
+    srv.cause_of_death AS "Cause of Death",
+    std.dbgap_accession AS "dbGaP Accession"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female';</t>
+  </si>
+  <si>
+    <t>SELECT
+    DISTINCT prt.participant_id AS "Participant Id",
+    trt.treatment_id AS "Treatment Id",
+    trt.age_at_treatment_start AS "Age at Treatment Start",
+    trt.age_at_treatment_end AS "Age at Treatment End",
+    trt.treatment_type AS "Treatment Type",
+    CONCAT('[', REPLACE(trt.treatment_agent, ';', ', '), ']') AS "Treatment Agent",
+    std.dbgap_accession AS "dbGaP Accession"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+    std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female'
+ORDER BY 
+    trt.treatment_id ASC
+LIMIT 100;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -356,14 +352,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -696,7 +689,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -727,10 +720,10 @@
     </row>
     <row r="2" spans="1:5" ht="297" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
@@ -754,35 +747,35 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>11</v>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -794,7 +787,7 @@
       <c r="C9" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Utils.py scripts to fix mapping issue
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC01_C3DC_phs002599_SexAtBirth-Female.xlsx
+++ b/InputFiles/C3DC/TC01_C3DC_phs002599_SexAtBirth-Female.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-09-25-2024/Commons_Automation/InputFiles/C3DC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-11-18-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A8115C-9D61-6D44-9905-90CDC9C803CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B555BC6-84F4-F545-A698-524DC7357D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="-2240" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-44380" yWindow="-2660" windowWidth="36800" windowHeight="26760" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -231,6 +231,28 @@
     std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female'</t>
   </si>
   <si>
+    <t>SELECT 
+    COUNT(DISTINCT dgn.diagnosis) AS Diagnoses,
+    COUNT(DISTINCT prt.participant_id) AS Participants,
+    COUNT(DISTINCT std.study_id) AS Studies
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+   std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female';</t>
+  </si>
+  <si>
     <t>SELECT
     DISTINCT prt.participant_id AS "Participant Id",
     trt.treatment_id AS "Treatment Id",
@@ -249,7 +271,7 @@
         trt.age_at_treatment_end 
 END AS "Age at Treatment End",
     trt.treatment_type AS "Treatment Type",
-    CONCAT(REPLACE(trt.treatment_agent, ';', ', ')) AS "Treatment Agent",
+    REPLACE(trt.treatment_agent, ';', ', ') AS "Treatment Agent",
     std.dbgap_accession AS "dbGaP Accession"
 FROM 
     df_study std
@@ -271,36 +293,21 @@
     trt.treatment_id ASC
 LIMIT 100;</t>
   </si>
-  <si>
-    <t>SELECT 
-    COUNT(DISTINCT dgn.diagnosis) AS Diagnoses,
-    COUNT(DISTINCT prt.participant_id) AS Participants,
-    COUNT(DISTINCT std.study_id) AS Studies
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
-WHERE 
-   std.dbgap_accession = 'phs002599' AND prt.sex_at_birth = 'Female';</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -360,11 +367,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -693,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -731,7 +741,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -761,8 +771,8 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -792,7 +802,7 @@
       <c r="C9" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>